<commit_message>
ajuste na geração dos gráficos
</commit_message>
<xml_diff>
--- a/xls/query_data.xlsx
+++ b/xls/query_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,71 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>idcg</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>nir_retrieved_relevants</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>nir_recall</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>nir_precision</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>nir_f_scores</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>nir_dcg</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>nir_ndcg</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>els_retrieved_relevants</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>els_recall</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>els_precision</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>els_f_scores</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>els_dcg</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>els_ndcg</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>system</t>
         </is>
       </c>
@@ -460,7 +525,46 @@
       <c r="C2" t="n">
         <v>29</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>24.7512662041</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="I2" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>6</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="O2" t="n">
+        <v>7.02</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>els / nir</t>
         </is>
@@ -476,7 +580,46 @@
       <c r="C3" t="n">
         <v>25</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>20.0373047392</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="O3" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>els / nir</t>
         </is>
@@ -490,9 +633,48 @@
         <v>33</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>14.7643646531</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>els</t>
         </is>
@@ -506,9 +688,48 @@
         <v>56</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="inlineStr">
+        <v>11</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.7363598161</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>els / nir</t>
         </is>
@@ -522,9 +743,48 @@
         <v>57</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D6" t="inlineStr">
+        <v>15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5.6670363741</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>els</t>
         </is>
@@ -538,9 +798,48 @@
         <v>83</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" t="inlineStr">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4.7363598161</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -554,9 +853,48 @@
         <v>99</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="inlineStr">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5.6670363741</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -572,7 +910,46 @@
       <c r="C9" t="n">
         <v>10</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>10.0101556221</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -586,9 +963,48 @@
         <v>109</v>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10.0101556221</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>els</t>
         </is>
@@ -602,9 +1018,48 @@
         <v>130</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3.2002531955</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>els</t>
         </is>
@@ -618,9 +1073,48 @@
         <v>171</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10.6768222888</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>els / nir</t>
         </is>
@@ -634,9 +1128,48 @@
         <v>189</v>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
-      </c>
-      <c r="D13" t="inlineStr">
+        <v>10</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10.6768222888</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -650,9 +1183,48 @@
         <v>196</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" t="inlineStr">
+        <v>13</v>
+      </c>
+      <c r="D14" t="n">
+        <v>15.4029424463</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>5</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="O14" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Q14" t="inlineStr">
         <is>
           <t>els</t>
         </is>
@@ -668,7 +1240,46 @@
       <c r="C15" t="n">
         <v>15</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>15.4029424463</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I15" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -682,9 +1293,48 @@
         <v>213</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
-      </c>
-      <c r="D16" t="inlineStr">
+        <v>12</v>
+      </c>
+      <c r="D16" t="n">
+        <v>10.9511272619</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>nir</t>
         </is>
@@ -698,9 +1348,48 @@
         <v>214</v>
       </c>
       <c r="C17" t="n">
-        <v>6</v>
-      </c>
-      <c r="D17" t="inlineStr">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10.9511272619</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>els / nir</t>
         </is>
@@ -714,9 +1403,48 @@
         <v>225</v>
       </c>
       <c r="C18" t="n">
-        <v>13</v>
-      </c>
-      <c r="D18" t="inlineStr">
+        <v>25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>22.6258604536</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="inlineStr">
         <is>
           <t>nir</t>
         </is>

</xml_diff>